<commit_message>
WorldID, ServerID 8비트로 변경
</commit_message>
<xml_diff>
--- a/Document/Data/Config/DummyClientConfig.xlsx
+++ b/Document/Data/Config/DummyClientConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HavePoop\Desktop\Study\Core\Document\Data\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6419EA7C-AE7D-4262-BB99-7745B8E1CFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03E327E-E3A6-4390-93D7-ACE480293C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="5280" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DummyClientConfig" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>WorldID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,6 +50,10 @@
   </si>
   <si>
     <t>MaxConnectionCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint8_t</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,7 +436,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -468,7 +472,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>

</xml_diff>